<commit_message>
Update template to match actual data columns
Campaign Data columns updated to match actual export:
- Date (A), Portfolio name (B), Campaign Name (D)
- Impressions (L), Clicks (N), Spend (Q)
- 7 Day Total Orders (U), 7 Day Total Sales (X)
- Portfolio Type (Y), Segment (Z), Week (AA), Month (AB)

Business Data columns updated to match actual export:
- Date (A), Ordered Product Sales (B), Units Ordered (D)
- Sessions - Total (N)
- Week (S), Month (T)

All SUMIFS formulas updated to reference correct columns.

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Campaign_Report_Template_v2.xlsx
+++ b/Campaign_Report_Template_v2.xlsx
@@ -39,7 +39,7 @@
     <numFmt numFmtId="169" formatCode="0.0%"/>
     <numFmt numFmtId="170" formatCode="0.00&quot;x&quot;"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="38">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -203,12 +203,17 @@
     <font>
       <b val="1"/>
       <color rgb="002E86AB"/>
-      <sz val="11"/>
+      <sz val="9"/>
     </font>
     <font>
       <b val="1"/>
       <color rgb="00F97316"/>
       <sz val="12"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00F97316"/>
+      <sz val="9"/>
     </font>
   </fonts>
   <fills count="11">
@@ -332,7 +337,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -473,6 +478,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -1429,11 +1435,11 @@
     </row>
     <row r="5">
       <c r="A5" s="23">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="B5" s="23">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="C5" s="68">
@@ -1445,11 +1451,11 @@
         <v/>
       </c>
       <c r="E5" s="69">
-        <f>SUMIFS('Campaign Data'!I:I,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!U:U,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="F5" s="69">
-        <f>SUMIFS('Campaign Data'!F:F,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!N:N,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="G5" s="70">
@@ -1498,11 +1504,11 @@
         </is>
       </c>
       <c r="B10" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN",'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN",'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="C10" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN",'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN",'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="D10" s="51">
@@ -1521,11 +1527,11 @@
         </is>
       </c>
       <c r="B11" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN",'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN",'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="C11" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN",'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN",'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="D11" s="51">
@@ -1544,11 +1550,11 @@
         </is>
       </c>
       <c r="B12" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN",'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN",'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="C12" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"JN",'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"JN",'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="D12" s="51">
@@ -1644,11 +1650,11 @@
     </row>
     <row r="5">
       <c r="A5" s="23">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="B5" s="23">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="C5" s="68">
@@ -1660,11 +1666,11 @@
         <v/>
       </c>
       <c r="E5" s="69">
-        <f>SUMIFS('Campaign Data'!I:I,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!U:U,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="F5" s="69">
-        <f>SUMIFS('Campaign Data'!F:F,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!N:N,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="G5" s="70">
@@ -1713,11 +1719,11 @@
         </is>
       </c>
       <c r="B10" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN",'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN",'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="C10" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN",'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN",'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="D10" s="51">
@@ -1736,11 +1742,11 @@
         </is>
       </c>
       <c r="B11" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN",'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN",'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="C11" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN",'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN",'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="D11" s="51">
@@ -1759,11 +1765,11 @@
         </is>
       </c>
       <c r="B12" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN",'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN",'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="C12" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,"Non-JN",'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,"Non-JN",'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="D12" s="51">
@@ -2497,7 +2503,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2505,24 +2511,34 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="12" customWidth="1" min="1" max="1"/>
-    <col width="20" customWidth="1" min="2" max="2"/>
-    <col width="40" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="12" customWidth="1" min="7" max="7"/>
-    <col width="14" customWidth="1" min="8" max="8"/>
-    <col width="14" customWidth="1" min="9" max="9"/>
-    <col width="12" customWidth="1" min="10" max="10"/>
-    <col width="12" customWidth="1" min="11" max="11"/>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="25" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="50" customWidth="1" min="4" max="4"/>
+    <col width="10" customWidth="1" min="5" max="5"/>
+    <col width="12" customWidth="1" min="6" max="6"/>
+    <col width="10" customWidth="1" min="7" max="7"/>
+    <col width="8" customWidth="1" min="8" max="8"/>
+    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="16" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
     <col width="12" customWidth="1" min="12" max="12"/>
-    <col width="14" customWidth="1" min="13" max="13"/>
-    <col width="14" customWidth="1" min="14" max="14"/>
-    <col width="12" customWidth="1" min="15" max="15"/>
-    <col width="14" customWidth="1" min="16" max="16"/>
+    <col width="12" customWidth="1" min="13" max="13"/>
+    <col width="10" customWidth="1" min="14" max="14"/>
+    <col width="10" customWidth="1" min="15" max="15"/>
+    <col width="12" customWidth="1" min="16" max="16"/>
     <col width="12" customWidth="1" min="17" max="17"/>
     <col width="12" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="12" customWidth="1" min="20" max="20"/>
+    <col width="14" customWidth="1" min="21" max="21"/>
+    <col width="14" customWidth="1" min="22" max="22"/>
+    <col width="14" customWidth="1" min="23" max="23"/>
+    <col width="14" customWidth="1" min="24" max="24"/>
+    <col width="12" customWidth="1" min="25" max="25"/>
+    <col width="14" customWidth="1" min="26" max="26"/>
+    <col width="12" customWidth="1" min="27" max="27"/>
+    <col width="12" customWidth="1" min="28" max="28"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2535,35 +2551,31 @@
     <row r="2">
       <c r="A2" s="7" t="inlineStr">
         <is>
-          <t>Format: Copy all data including headers from your CSV export</t>
+          <t>Format: Copy all data including headers from your CSV export (row 4 shows expected columns)</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="75" t="inlineStr">
         <is>
-          <t>Data Table:</t>
-        </is>
-      </c>
-      <c r="O3" s="76" t="inlineStr">
-        <is>
-          <t>Formula: =IF(ISNUMBER(SEARCH("JN",B5)),"JN","Non-JN")</t>
-        </is>
-      </c>
-      <c r="P3" s="76" t="inlineStr">
-        <is>
-          <t>Formula: =IF(ISNUMBER(SEARCH("branded",C5)),"Branded",IF(OR(ISNUMBER(SEARCH(" pat ",C5)),ISNUMBER(SEARCH("- pat -",C5))),"Competitor","Non-Branded"))</t>
-        </is>
-      </c>
-      <c r="Q3" s="76" t="inlineStr">
-        <is>
-          <t>Formula: =TEXT(A5,"YYYY")"-W"&amp;TEXT(WEEKNUM(A5),"00")</t>
-        </is>
-      </c>
-      <c r="R3" s="76" t="inlineStr">
-        <is>
-          <t>Formula: =TEXT(A5,"MMM YYYY")</t>
-        </is>
+          <t>Key columns: A=Date, B=Portfolio, D=Campaign, L=Impressions, N=Clicks, Q=Spend, X=Sales, U=Orders</t>
+        </is>
+      </c>
+      <c r="Y3" s="76">
+        <f>IF(ISNUMBER(SEARCH("JN",B5)),"JN","Non-JN")</f>
+        <v/>
+      </c>
+      <c r="Z3" s="76">
+        <f>IF(ISNUMBER(SEARCH("branded",D5)),"Branded",IF(OR(ISNUMBER(SEARCH(" pat ",D5)),ISNUMBER(SEARCH("- pat -",D5))),"Competitor","Non-Branded"))</f>
+        <v/>
+      </c>
+      <c r="AA3" s="76">
+        <f>TEXT(A5,"YYYY")"-W"&amp;TEXT(WEEKNUM(A5),"00")</f>
+        <v/>
+      </c>
+      <c r="AB3" s="76">
+        <f>TEXT(A5,"MMM YYYY")</f>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -2579,80 +2591,130 @@
       </c>
       <c r="C4" s="5" t="inlineStr">
         <is>
+          <t>Program Type</t>
+        </is>
+      </c>
+      <c r="D4" s="5" t="inlineStr">
+        <is>
           <t>Campaign Name</t>
         </is>
       </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>Ad Group Name</t>
-        </is>
-      </c>
       <c r="E4" s="5" t="inlineStr">
         <is>
+          <t>Retailer</t>
+        </is>
+      </c>
+      <c r="F4" s="5" t="inlineStr">
+        <is>
+          <t>Country</t>
+        </is>
+      </c>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+      <c r="H4" s="5" t="inlineStr">
+        <is>
+          <t>Currency</t>
+        </is>
+      </c>
+      <c r="I4" s="5" t="inlineStr">
+        <is>
+          <t>Budget Amount</t>
+        </is>
+      </c>
+      <c r="J4" s="5" t="inlineStr">
+        <is>
+          <t>Targeting Type</t>
+        </is>
+      </c>
+      <c r="K4" s="5" t="inlineStr">
+        <is>
+          <t>Bidding strategy</t>
+        </is>
+      </c>
+      <c r="L4" s="5" t="inlineStr">
+        <is>
           <t>Impressions</t>
         </is>
       </c>
-      <c r="F4" s="5" t="inlineStr">
+      <c r="M4" s="5" t="inlineStr">
+        <is>
+          <t>Last Year Impressions</t>
+        </is>
+      </c>
+      <c r="N4" s="5" t="inlineStr">
         <is>
           <t>Clicks</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="O4" s="5" t="inlineStr">
+        <is>
+          <t>Last Year Clicks</t>
+        </is>
+      </c>
+      <c r="P4" s="5" t="inlineStr">
+        <is>
+          <t>Click-Thru Rate (CTR)</t>
+        </is>
+      </c>
+      <c r="Q4" s="5" t="inlineStr">
         <is>
           <t>Spend</t>
         </is>
       </c>
-      <c r="H4" s="5" t="inlineStr">
-        <is>
-          <t>7 Day Total Sales</t>
-        </is>
-      </c>
-      <c r="I4" s="5" t="inlineStr">
+      <c r="R4" s="5" t="inlineStr">
+        <is>
+          <t>Last Year Spend</t>
+        </is>
+      </c>
+      <c r="S4" s="5" t="inlineStr">
+        <is>
+          <t>Cost Per Click (CPC)</t>
+        </is>
+      </c>
+      <c r="T4" s="5" t="inlineStr">
+        <is>
+          <t>Last Year Cost Per Click (CPC)</t>
+        </is>
+      </c>
+      <c r="U4" s="5" t="inlineStr">
         <is>
           <t>7 Day Total Orders (#)</t>
         </is>
       </c>
-      <c r="J4" s="5" t="inlineStr">
-        <is>
-          <t>7 Day Conversion Rate</t>
-        </is>
-      </c>
-      <c r="K4" s="5" t="inlineStr">
-        <is>
-          <t>Cost Per Click (CPC)</t>
-        </is>
-      </c>
-      <c r="L4" s="5" t="inlineStr">
-        <is>
-          <t>Click-Thru Rate (CTR)</t>
-        </is>
-      </c>
-      <c r="M4" s="5" t="inlineStr">
-        <is>
-          <t>7 Day Advertised SKU Sales</t>
-        </is>
-      </c>
-      <c r="N4" s="5" t="inlineStr">
-        <is>
-          <t>7 Day Other SKU Sales</t>
-        </is>
-      </c>
-      <c r="O4" s="5" t="inlineStr">
+      <c r="V4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Total Advertising Cost of Sales (ACOS) </t>
+        </is>
+      </c>
+      <c r="W4" s="5" t="inlineStr">
+        <is>
+          <t>Total Return on Advertising Spend (ROAS)</t>
+        </is>
+      </c>
+      <c r="X4" s="5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">7 Day Total Sales </t>
+        </is>
+      </c>
+      <c r="Y4" s="5" t="inlineStr">
         <is>
           <t>Portfolio Type</t>
         </is>
       </c>
-      <c r="P4" s="5" t="inlineStr">
+      <c r="Z4" s="5" t="inlineStr">
         <is>
           <t>Segment</t>
         </is>
       </c>
-      <c r="Q4" s="5" t="inlineStr">
+      <c r="AA4" s="5" t="inlineStr">
         <is>
           <t>Week</t>
         </is>
       </c>
-      <c r="R4" s="5" t="inlineStr">
+      <c r="AB4" s="5" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
@@ -2660,7 +2722,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:R1"/>
+    <mergeCell ref="A1:Z1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2672,7 +2734,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2682,13 +2744,24 @@
   <cols>
     <col width="12" customWidth="1" min="1" max="1"/>
     <col width="18" customWidth="1" min="2" max="2"/>
-    <col width="14" customWidth="1" min="3" max="3"/>
-    <col width="12" customWidth="1" min="4" max="4"/>
-    <col width="12" customWidth="1" min="5" max="5"/>
-    <col width="16" customWidth="1" min="6" max="6"/>
-    <col width="18" customWidth="1" min="7" max="7"/>
-    <col width="12" customWidth="1" min="8" max="8"/>
-    <col width="12" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="14" customWidth="1" min="4" max="4"/>
+    <col width="14" customWidth="1" min="5" max="5"/>
+    <col width="14" customWidth="1" min="6" max="6"/>
+    <col width="14" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+    <col width="18" customWidth="1" min="9" max="9"/>
+    <col width="18" customWidth="1" min="10" max="10"/>
+    <col width="18" customWidth="1" min="11" max="11"/>
+    <col width="16" customWidth="1" min="12" max="12"/>
+    <col width="16" customWidth="1" min="13" max="13"/>
+    <col width="14" customWidth="1" min="14" max="14"/>
+    <col width="14" customWidth="1" min="15" max="15"/>
+    <col width="20" customWidth="1" min="16" max="16"/>
+    <col width="20" customWidth="1" min="17" max="17"/>
+    <col width="16" customWidth="1" min="18" max="18"/>
+    <col width="12" customWidth="1" min="19" max="19"/>
+    <col width="12" customWidth="1" min="20" max="20"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2706,15 +2779,18 @@
       </c>
     </row>
     <row r="3">
-      <c r="H3" s="76" t="inlineStr">
-        <is>
-          <t>Formula: =TEXT(A5,"YYYY")"-W"&amp;TEXT(WEEKNUM(A5),"00")</t>
-        </is>
-      </c>
-      <c r="I3" s="76" t="inlineStr">
-        <is>
-          <t>Formula: =TEXT(A5,"MMM YYYY")</t>
-        </is>
+      <c r="A3" s="78" t="inlineStr">
+        <is>
+          <t>Key columns: A=Date, B=Ordered Product Sales (Total Sales), D=Units Ordered, N=Sessions</t>
+        </is>
+      </c>
+      <c r="S3" s="76">
+        <f>TEXT(A5,"YYYY")"-W"&amp;TEXT(WEEKNUM(A5),"00")</f>
+        <v/>
+      </c>
+      <c r="T3" s="76">
+        <f>TEXT(A5,"MMM YYYY")</f>
+        <v/>
       </c>
     </row>
     <row r="4">
@@ -2730,35 +2806,90 @@
       </c>
       <c r="C4" s="66" t="inlineStr">
         <is>
+          <t>Ordered Product Sales - B2B</t>
+        </is>
+      </c>
+      <c r="D4" s="66" t="inlineStr">
+        <is>
           <t>Units Ordered</t>
         </is>
       </c>
-      <c r="D4" s="66" t="inlineStr">
-        <is>
-          <t>Sessions</t>
-        </is>
-      </c>
       <c r="E4" s="66" t="inlineStr">
         <is>
-          <t>Page Views</t>
+          <t>Units Ordered - B2B</t>
         </is>
       </c>
       <c r="F4" s="66" t="inlineStr">
         <is>
-          <t>Session Percentage</t>
+          <t>Total Order Items</t>
         </is>
       </c>
       <c r="G4" s="66" t="inlineStr">
         <is>
-          <t>Unit Session Percentage</t>
+          <t>Total Order Items - B2B</t>
         </is>
       </c>
       <c r="H4" s="66" t="inlineStr">
         <is>
+          <t>Average Sales per Order Item</t>
+        </is>
+      </c>
+      <c r="I4" s="66" t="inlineStr">
+        <is>
+          <t>Average Sales per Order Item - B2B</t>
+        </is>
+      </c>
+      <c r="J4" s="66" t="inlineStr">
+        <is>
+          <t>Average Units per Order Item</t>
+        </is>
+      </c>
+      <c r="K4" s="66" t="inlineStr">
+        <is>
+          <t>Average Units per Order Item - B2B</t>
+        </is>
+      </c>
+      <c r="L4" s="66" t="inlineStr">
+        <is>
+          <t>Average Selling Price</t>
+        </is>
+      </c>
+      <c r="M4" s="66" t="inlineStr">
+        <is>
+          <t>Average Selling Price - B2B</t>
+        </is>
+      </c>
+      <c r="N4" s="66" t="inlineStr">
+        <is>
+          <t>Sessions - Total</t>
+        </is>
+      </c>
+      <c r="O4" s="66" t="inlineStr">
+        <is>
+          <t>Sessions - Total - B2B</t>
+        </is>
+      </c>
+      <c r="P4" s="66" t="inlineStr">
+        <is>
+          <t>Order Item Session Percentage</t>
+        </is>
+      </c>
+      <c r="Q4" s="66" t="inlineStr">
+        <is>
+          <t>Order Item Session Percentage - B2B</t>
+        </is>
+      </c>
+      <c r="R4" s="66" t="inlineStr">
+        <is>
+          <t>Average Offer Count</t>
+        </is>
+      </c>
+      <c r="S4" s="66" t="inlineStr">
+        <is>
           <t>Week</t>
         </is>
       </c>
-      <c r="I4" s="66" t="inlineStr">
+      <c r="T4" s="66" t="inlineStr">
         <is>
           <t>Month</t>
         </is>
@@ -2766,7 +2897,7 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:S1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -2866,7 +2997,7 @@
     </row>
     <row r="9">
       <c r="A9" s="15">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!O:O,IF(Settings!B4="Overall","*",IF(Settings!B4="JN","JN","Non-JN")))</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Y:Y,IF(Settings!B4="Overall","*",IF(Settings!B4="JN","JN","Non-JN")))</f>
         <v/>
       </c>
     </row>
@@ -3011,11 +3142,11 @@
         </is>
       </c>
       <c r="B20" s="26">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="C20" s="26">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="D20" s="27">
@@ -3034,11 +3165,11 @@
         </is>
       </c>
       <c r="B21" s="26">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="C21" s="26">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="D21" s="27">
@@ -3057,11 +3188,11 @@
         </is>
       </c>
       <c r="B22" s="26">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="C22" s="26">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="D22" s="27">
@@ -3411,7 +3542,7 @@
         </is>
       </c>
       <c r="B6" s="32" t="n">
-        <v>45940.80602209453</v>
+        <v>45940.83268908651</v>
       </c>
     </row>
     <row r="7">
@@ -3421,7 +3552,7 @@
         </is>
       </c>
       <c r="B7" s="32" t="n">
-        <v>46030.80602209592</v>
+        <v>46030.83268908819</v>
       </c>
     </row>
     <row r="10">
@@ -3511,7 +3642,7 @@
         </is>
       </c>
       <c r="B17" s="33" t="n">
-        <v>46030.80602209768</v>
+        <v>46030.83268909029</v>
       </c>
     </row>
     <row r="18">
@@ -3610,11 +3741,11 @@
     </row>
     <row r="6">
       <c r="A6" s="36">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!R:R,TEXT(EOMONTH(Settings!B7,-1)+1,"MMM YYYY"))</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!AB:AB,TEXT(EOMONTH(Settings!B7,-1)+1,"MMM YYYY"))</f>
         <v/>
       </c>
       <c r="E6" s="26">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!R:R,TEXT(EOMONTH(Settings!B7,-2)+1,"MMM YYYY"))</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!AB:AB,TEXT(EOMONTH(Settings!B7,-2)+1,"MMM YYYY"))</f>
         <v/>
       </c>
     </row>
@@ -3648,11 +3779,11 @@
     </row>
     <row r="10">
       <c r="A10" s="38">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!R:R,TEXT(EOMONTH(Settings!B7,-1)+1,"MMM YYYY"))</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!R:R,TEXT(EOMONTH(Settings!B7,-1)+1,"MMM YYYY"))</f>
         <v/>
       </c>
       <c r="C10" s="38">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!R:R,TEXT(EOMONTH(Settings!B7,-1)+1,"MMM YYYY"))</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!R:R,TEXT(EOMONTH(Settings!B7,-1)+1,"MMM YYYY"))</f>
         <v/>
       </c>
       <c r="E10" s="39">
@@ -4000,7 +4131,7 @@
         </is>
       </c>
       <c r="B6" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="C6" s="50">
@@ -4008,7 +4139,7 @@
         <v/>
       </c>
       <c r="D6" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded")</f>
         <v/>
       </c>
       <c r="E6" s="50">
@@ -4033,7 +4164,7 @@
         </is>
       </c>
       <c r="B7" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="C7" s="50">
@@ -4041,7 +4172,7 @@
         <v/>
       </c>
       <c r="D7" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor")</f>
         <v/>
       </c>
       <c r="E7" s="50">
@@ -4066,7 +4197,7 @@
         </is>
       </c>
       <c r="B8" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="C8" s="50">
@@ -4074,7 +4205,7 @@
         <v/>
       </c>
       <c r="D8" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded")</f>
         <v/>
       </c>
       <c r="E8" s="50">
@@ -4178,11 +4309,11 @@
         </is>
       </c>
       <c r="B14" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded",'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded",'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="C14" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded",'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded",'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="D14" s="51">
@@ -4190,11 +4321,11 @@
         <v/>
       </c>
       <c r="E14" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded",'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded",'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="F14" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Branded",'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Branded",'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="G14" s="51">
@@ -4209,11 +4340,11 @@
         </is>
       </c>
       <c r="B15" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor",'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor",'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="C15" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor",'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor",'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="D15" s="51">
@@ -4221,11 +4352,11 @@
         <v/>
       </c>
       <c r="E15" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor",'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor",'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="F15" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Competitor",'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Competitor",'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="G15" s="51">
@@ -4240,11 +4371,11 @@
         </is>
       </c>
       <c r="B16" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded",'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded",'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="C16" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded",'Campaign Data'!O:O,"JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded",'Campaign Data'!Y:Y,"JN")</f>
         <v/>
       </c>
       <c r="D16" s="51">
@@ -4252,11 +4383,11 @@
         <v/>
       </c>
       <c r="E16" s="49">
-        <f>SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded",'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded",'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="F16" s="49">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!P:P,"Non-Branded",'Campaign Data'!O:O,"Non-JN")</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7,'Campaign Data'!Z:Z,"Non-Branded",'Campaign Data'!Y:Y,"Non-JN")</f>
         <v/>
       </c>
       <c r="G16" s="51">
@@ -5475,7 +5606,7 @@
         <v/>
       </c>
       <c r="B6" s="23">
-        <f>SUMIFS('Campaign Data'!H:H,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7)</f>
+        <f>SUMIFS('Campaign Data'!X:X,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7)</f>
         <v/>
       </c>
       <c r="C6" s="23">
@@ -5491,7 +5622,7 @@
         <v/>
       </c>
       <c r="F6" s="24">
-        <f>IF(A6&gt;0,SUMIFS('Campaign Data'!G:G,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7)/A6,0)</f>
+        <f>IF(A6&gt;0,SUMIFS('Campaign Data'!Q:Q,'Campaign Data'!A:A,"&gt;="&amp;Settings!B6,'Campaign Data'!A:A,"&lt;="&amp;Settings!B7)/A6,0)</f>
         <v/>
       </c>
     </row>

</xml_diff>